<commit_message>
Actualizar import con años
Actualizar caja con años.
</commit_message>
<xml_diff>
--- a/Tasas/caja/caja.xlsx
+++ b/Tasas/caja/caja.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4295" uniqueCount="2029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4304" uniqueCount="2038">
   <si>
     <t>id</t>
   </si>
@@ -4163,42 +4163,63 @@
     <t>arch</t>
   </si>
   <si>
+    <t>value</t>
+  </si>
+  <si>
     <t>https://github.com/AlfCano/enoe/raw/devel/Salidas/ENOE2017_3t_SCC.RData</t>
   </si>
   <si>
     <t>sc3t2017</t>
   </si>
   <si>
+    <t>2017</t>
+  </si>
+  <si>
     <t>https://github.com/AlfCano/enoe/raw/devel/Salidas/ENOE2018_3t_SCC.RData</t>
   </si>
   <si>
     <t>sc3t2018</t>
   </si>
   <si>
+    <t>2018</t>
+  </si>
+  <si>
     <t>https://github.com/AlfCano/enoe/raw/devel/Salidas/ENOE2019_3t_SCC.RData</t>
   </si>
   <si>
     <t>sc3t2019</t>
   </si>
   <si>
+    <t>2019</t>
+  </si>
+  <si>
     <t>https://github.com/AlfCano/enoe/raw/devel/Salidas/ENOE2020_3t_SCC.RData</t>
   </si>
   <si>
     <t>sc3t2020</t>
   </si>
   <si>
+    <t>2020</t>
+  </si>
+  <si>
     <t>https://github.com/AlfCano/enoe/raw/devel/Salidas/ENOE2021_3t_SCC.RData</t>
   </si>
   <si>
     <t>sc3t2021</t>
   </si>
   <si>
+    <t>2021</t>
+  </si>
+  <si>
     <t>https://github.com/AlfCano/enoe/raw/devel/Salidas/ENOE2022_3t_SCC.RData</t>
   </si>
   <si>
     <t>sc3t2022</t>
   </si>
   <si>
+    <t>2022</t>
+  </si>
+  <si>
     <t>df</t>
   </si>
   <si>
@@ -6099,6 +6120,12 @@
   </si>
   <si>
     <t>p4d2_1</t>
+  </si>
+  <si>
+    <t>ent.z</t>
+  </si>
+  <si>
+    <t>Zona de Entidad</t>
   </si>
   <si>
     <t>https://github.com/AlfCano/enoe/raw/devel/Tasas/Utils/meta_sd_cs.RData</t>
@@ -6150,7 +6177,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -6159,6 +6186,9 @@
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -18316,7 +18346,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="98.63"/>
+    <col customWidth="1" min="1" max="1" width="66.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -18326,53 +18356,74 @@
       <c r="B1" s="1" t="s">
         <v>384</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>1381</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1382</v>
+        <v>1383</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1384</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>1383</v>
+        <v>1385</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1384</v>
+        <v>1386</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1387</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>1385</v>
+        <v>1388</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1386</v>
+        <v>1389</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1390</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>1387</v>
+        <v>1391</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1393</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>1389</v>
+        <v>1394</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1390</v>
+        <v>1395</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1396</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>1391</v>
+        <v>1397</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1392</v>
+        <v>1398</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1399</v>
       </c>
     </row>
   </sheetData>
@@ -18395,255 +18446,255 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1393</v>
+        <v>1400</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1394</v>
+        <v>1401</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1395</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>1386</v>
+        <v>1389</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1396</v>
+        <v>1403</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1397</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>1386</v>
+        <v>1389</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1398</v>
+        <v>1405</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1399</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1400</v>
+        <v>1407</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1401</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1402</v>
+        <v>1409</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>1403</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1404</v>
+        <v>1411</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1405</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1406</v>
+        <v>1413</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1407</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1408</v>
+        <v>1415</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>1409</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1410</v>
+        <v>1417</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>1411</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1412</v>
+        <v>1419</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1413</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1414</v>
+        <v>1421</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>1415</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1416</v>
+        <v>1423</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1417</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1418</v>
+        <v>1425</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>1419</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1420</v>
+        <v>1427</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>1421</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1422</v>
+        <v>1429</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>1423</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1424</v>
+        <v>1431</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>1425</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1426</v>
+        <v>1433</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>1427</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1428</v>
+        <v>1435</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>1429</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1430</v>
+        <v>1437</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>1431</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1432</v>
+        <v>1439</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>1433</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>1390</v>
+        <v>1395</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1434</v>
+        <v>1441</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>1435</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>1390</v>
+        <v>1395</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1400</v>
+        <v>1407</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>1401</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>1392</v>
+        <v>1398</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1434</v>
+        <v>1441</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>1435</v>
+        <v>1442</v>
       </c>
     </row>
   </sheetData>
@@ -18666,7 +18717,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1394</v>
+        <v>1401</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -18674,74 +18725,74 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>1436</v>
+        <v>1443</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1437</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>1438</v>
+        <v>1445</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1439</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>1440</v>
+        <v>1447</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1441</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>1442</v>
+        <v>1449</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1443</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>1444</v>
+        <v>1451</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1445</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>1446</v>
+        <v>1453</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1447</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>1448</v>
+        <v>1455</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1449</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>1450</v>
+        <v>1457</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1451</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>1452</v>
+        <v>1459</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1453</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="11">
@@ -18749,7 +18800,7 @@
         <v>385</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1454</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="12">
@@ -18757,103 +18808,103 @@
         <v>387</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1455</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>1456</v>
+        <v>1463</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1457</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>1458</v>
+        <v>1465</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1459</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>1460</v>
+        <v>1467</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1461</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>1462</v>
+        <v>1469</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1463</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>1464</v>
+        <v>1471</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1465</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>1466</v>
+        <v>1473</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1467</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>1468</v>
+        <v>1475</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1469</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>1470</v>
+        <v>1477</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1471</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>1472</v>
+        <v>1479</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1473</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>1474</v>
+        <v>1481</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1475</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>1476</v>
+        <v>1483</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1477</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>1478</v>
+        <v>1485</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1479</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="25">
@@ -18861,231 +18912,231 @@
         <v>393</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1480</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>1481</v>
+        <v>1488</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1482</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>1483</v>
+        <v>1490</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1484</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>1485</v>
+        <v>1492</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1486</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>1487</v>
+        <v>1494</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1488</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>1434</v>
+        <v>1441</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1435</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>1489</v>
+        <v>1496</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>1490</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>1491</v>
+        <v>1498</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1492</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>1493</v>
+        <v>1500</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1492</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>1494</v>
+        <v>1501</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1495</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>1496</v>
+        <v>1503</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1497</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>1498</v>
+        <v>1505</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1499</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>1500</v>
+        <v>1507</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1501</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
-        <v>1502</v>
+        <v>1509</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1503</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>1504</v>
+        <v>1511</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>1505</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>1506</v>
+        <v>1513</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1507</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>1508</v>
+        <v>1515</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1509</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>1510</v>
+        <v>1517</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1511</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>1512</v>
+        <v>1519</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1513</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="s">
-        <v>1514</v>
+        <v>1521</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1515</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>1516</v>
+        <v>1523</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1517</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>1518</v>
+        <v>1525</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1519</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>1520</v>
+        <v>1527</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>1521</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
-        <v>1522</v>
+        <v>1529</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1523</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="s">
-        <v>1524</v>
+        <v>1531</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1525</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
-        <v>1526</v>
+        <v>1533</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1527</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>1528</v>
+        <v>1535</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1529</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
-        <v>1530</v>
+        <v>1537</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>1531</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
-        <v>1532</v>
+        <v>1539</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>1533</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="54">
@@ -19093,15 +19144,15 @@
         <v>395</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>1534</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
-        <v>1535</v>
+        <v>1542</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1536</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="56">
@@ -19109,7 +19160,7 @@
         <v>80</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>1537</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="57">
@@ -19117,15 +19168,15 @@
         <v>65</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1538</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="s">
-        <v>1539</v>
+        <v>1546</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1540</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="59">
@@ -19133,71 +19184,71 @@
         <v>184</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1541</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
-        <v>1542</v>
+        <v>1549</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>1543</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="s">
-        <v>1544</v>
+        <v>1551</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>1545</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
-        <v>1546</v>
+        <v>1553</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>1547</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="s">
-        <v>1548</v>
+        <v>1555</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>1549</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="s">
-        <v>1550</v>
+        <v>1557</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>1551</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="s">
-        <v>1552</v>
+        <v>1559</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>1553</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="s">
-        <v>1554</v>
+        <v>1561</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>1555</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="s">
-        <v>1556</v>
+        <v>1563</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>1557</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="68">
@@ -19205,7 +19256,7 @@
         <v>91</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>1558</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="69">
@@ -19213,103 +19264,103 @@
         <v>113</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1559</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="s">
-        <v>1560</v>
+        <v>1567</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>1561</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="s">
-        <v>1562</v>
+        <v>1569</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>1563</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="s">
-        <v>1564</v>
+        <v>1571</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>1565</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="s">
-        <v>1566</v>
+        <v>1573</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>1567</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="s">
-        <v>1568</v>
+        <v>1575</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>1569</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="s">
-        <v>1570</v>
+        <v>1577</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>1571</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="s">
-        <v>1572</v>
+        <v>1579</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>1573</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="s">
-        <v>1574</v>
+        <v>1581</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>1575</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="s">
-        <v>1576</v>
+        <v>1583</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>1577</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="s">
-        <v>1578</v>
+        <v>1585</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>1579</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="s">
-        <v>1580</v>
+        <v>1587</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>1581</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="s">
-        <v>1582</v>
+        <v>1589</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>1583</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="82">
@@ -19317,7 +19368,7 @@
         <v>208</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>1584</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="83">
@@ -19325,7 +19376,7 @@
         <v>223</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>1585</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="84">
@@ -19333,223 +19384,223 @@
         <v>242</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>1586</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="s">
-        <v>1587</v>
+        <v>1594</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>1588</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="s">
-        <v>1589</v>
+        <v>1596</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>1590</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="s">
-        <v>1591</v>
+        <v>1598</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>1592</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="s">
-        <v>1593</v>
+        <v>1600</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>1594</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="s">
-        <v>1595</v>
+        <v>1602</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>1596</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="s">
-        <v>1597</v>
+        <v>1604</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>1598</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3" t="s">
-        <v>1599</v>
+        <v>1606</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>1600</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="3" t="s">
-        <v>1601</v>
+        <v>1608</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>1602</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="3" t="s">
-        <v>1603</v>
+        <v>1610</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>1604</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="3" t="s">
-        <v>1605</v>
+        <v>1612</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>1606</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="3" t="s">
-        <v>1607</v>
+        <v>1614</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>1608</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="3" t="s">
-        <v>1609</v>
+        <v>1616</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1610</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="3" t="s">
-        <v>1611</v>
+        <v>1618</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1612</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="3" t="s">
-        <v>1613</v>
+        <v>1620</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>1614</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="3" t="s">
-        <v>1615</v>
+        <v>1622</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>1616</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="3" t="s">
-        <v>1617</v>
+        <v>1624</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>1618</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="3" t="s">
-        <v>1619</v>
+        <v>1626</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>1620</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="3" t="s">
-        <v>1621</v>
+        <v>1628</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>1622</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="3" t="s">
-        <v>1623</v>
+        <v>1630</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>1624</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="3" t="s">
-        <v>1625</v>
+        <v>1632</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>1626</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="3" t="s">
-        <v>1627</v>
+        <v>1634</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>1628</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="3" t="s">
-        <v>1629</v>
+        <v>1636</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>1630</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="3" t="s">
-        <v>1631</v>
+        <v>1638</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>1632</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="3" t="s">
-        <v>1633</v>
+        <v>1640</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>1634</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="3" t="s">
-        <v>1635</v>
+        <v>1642</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1636</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="3" t="s">
-        <v>1637</v>
+        <v>1644</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>1638</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="3" t="s">
-        <v>1639</v>
+        <v>1646</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>1640</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="112">
@@ -19557,7 +19608,7 @@
         <v>270</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>1641</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="113">
@@ -19565,1767 +19616,1775 @@
         <v>8</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1642</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="3" t="s">
-        <v>1643</v>
+        <v>1650</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>1644</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="3" t="s">
-        <v>1645</v>
+        <v>1652</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>1646</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="3" t="s">
-        <v>1647</v>
+        <v>1654</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>1648</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="3" t="s">
-        <v>1649</v>
+        <v>1656</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>1650</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="3" t="s">
-        <v>1651</v>
+        <v>1658</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>1652</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="3" t="s">
-        <v>1653</v>
+        <v>1660</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>1654</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="3" t="s">
-        <v>1655</v>
+        <v>1662</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>1656</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="3" t="s">
-        <v>1657</v>
+        <v>1664</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>1658</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="3" t="s">
-        <v>1659</v>
+        <v>1666</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>1660</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="3" t="s">
-        <v>1661</v>
+        <v>1668</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>1662</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="3" t="s">
-        <v>1663</v>
+        <v>1670</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>1664</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="3" t="s">
-        <v>1665</v>
+        <v>1672</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>1666</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="3" t="s">
-        <v>1667</v>
+        <v>1674</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>1668</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="3" t="s">
-        <v>1669</v>
+        <v>1676</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>1670</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="3" t="s">
-        <v>1671</v>
+        <v>1678</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>1672</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="3" t="s">
-        <v>1673</v>
+        <v>1680</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>1674</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="3" t="s">
-        <v>1675</v>
+        <v>1682</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>1676</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="3" t="s">
-        <v>1677</v>
+        <v>1684</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>1678</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="3" t="s">
-        <v>1679</v>
+        <v>1686</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>1680</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="3" t="s">
-        <v>1681</v>
+        <v>1688</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>1682</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="3" t="s">
-        <v>1683</v>
+        <v>1690</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>1684</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="3" t="s">
-        <v>1685</v>
+        <v>1692</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>1686</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="3" t="s">
-        <v>1687</v>
+        <v>1694</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>1688</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="3" t="s">
-        <v>1689</v>
+        <v>1696</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>1690</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="3" t="s">
-        <v>1691</v>
+        <v>1698</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>1692</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="3" t="s">
-        <v>1693</v>
+        <v>1700</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>1694</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="3" t="s">
-        <v>1695</v>
+        <v>1702</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>1696</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="3" t="s">
-        <v>1697</v>
+        <v>1704</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1698</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="3" t="s">
-        <v>1699</v>
+        <v>1706</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1700</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="3" t="s">
-        <v>1701</v>
+        <v>1708</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>1702</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="3" t="s">
-        <v>1703</v>
+        <v>1710</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>1704</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="3" t="s">
-        <v>1705</v>
+        <v>1712</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1706</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="3" t="s">
-        <v>1707</v>
+        <v>1714</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1708</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="3" t="s">
-        <v>1709</v>
+        <v>1716</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1710</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="3" t="s">
-        <v>1711</v>
+        <v>1718</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1712</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="3" t="s">
-        <v>1713</v>
+        <v>1720</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1714</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="3" t="s">
-        <v>1715</v>
+        <v>1722</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1716</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="3" t="s">
-        <v>1717</v>
+        <v>1724</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1718</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="3" t="s">
-        <v>1719</v>
+        <v>1726</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1720</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="3" t="s">
-        <v>1721</v>
+        <v>1728</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1722</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="3" t="s">
-        <v>1723</v>
+        <v>1730</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1724</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="3" t="s">
-        <v>1725</v>
+        <v>1732</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1726</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="3" t="s">
-        <v>1727</v>
+        <v>1734</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1728</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="3" t="s">
-        <v>1729</v>
+        <v>1736</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1730</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="3" t="s">
-        <v>1731</v>
+        <v>1738</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1732</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="3" t="s">
-        <v>1733</v>
+        <v>1740</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1734</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="3" t="s">
-        <v>1735</v>
+        <v>1742</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1736</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="3" t="s">
-        <v>1737</v>
+        <v>1744</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1738</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="3" t="s">
-        <v>1739</v>
+        <v>1746</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1740</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="3" t="s">
-        <v>1741</v>
+        <v>1748</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1742</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="3" t="s">
-        <v>1743</v>
+        <v>1750</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1744</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="3" t="s">
-        <v>1745</v>
+        <v>1752</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1746</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="3" t="s">
-        <v>1747</v>
+        <v>1754</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1748</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="3" t="s">
-        <v>1749</v>
+        <v>1756</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1750</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="3" t="s">
-        <v>1751</v>
+        <v>1758</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1752</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="3" t="s">
-        <v>1753</v>
+        <v>1760</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1754</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="3" t="s">
-        <v>1755</v>
+        <v>1762</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1756</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="3" t="s">
-        <v>1757</v>
+        <v>1764</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1758</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="3" t="s">
-        <v>1759</v>
+        <v>1766</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1760</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="3" t="s">
-        <v>1761</v>
+        <v>1768</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1762</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="3" t="s">
-        <v>1763</v>
+        <v>1770</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1764</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="3" t="s">
-        <v>1765</v>
+        <v>1772</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1766</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="3" t="s">
-        <v>1767</v>
+        <v>1774</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1768</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="3" t="s">
-        <v>1769</v>
+        <v>1776</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>1770</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="3" t="s">
-        <v>1396</v>
+        <v>1403</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1397</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="3" t="s">
-        <v>1771</v>
+        <v>1778</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1772</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="3" t="s">
-        <v>1773</v>
+        <v>1780</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1774</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="3" t="s">
-        <v>1775</v>
+        <v>1782</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1776</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="3" t="s">
-        <v>1777</v>
+        <v>1784</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1778</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="3" t="s">
-        <v>1779</v>
+        <v>1786</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1780</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="3" t="s">
-        <v>1781</v>
+        <v>1788</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1782</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="3" t="s">
-        <v>1783</v>
+        <v>1790</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1784</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="3" t="s">
-        <v>1785</v>
+        <v>1792</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1786</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="3" t="s">
-        <v>1787</v>
+        <v>1794</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1788</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="3" t="s">
-        <v>1789</v>
+        <v>1796</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1790</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="3" t="s">
-        <v>1791</v>
+        <v>1798</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>1792</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="3" t="s">
-        <v>1793</v>
+        <v>1800</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1794</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="3" t="s">
-        <v>1795</v>
+        <v>1802</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1796</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="3" t="s">
-        <v>1797</v>
+        <v>1804</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>1798</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="3" t="s">
-        <v>1799</v>
+        <v>1806</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1800</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="3" t="s">
-        <v>1801</v>
+        <v>1808</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1802</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="3" t="s">
-        <v>1803</v>
+        <v>1810</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1804</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="3" t="s">
-        <v>1805</v>
+        <v>1812</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1806</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="3" t="s">
-        <v>1807</v>
+        <v>1814</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1808</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="3" t="s">
-        <v>1809</v>
+        <v>1816</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1810</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="3" t="s">
-        <v>1811</v>
+        <v>1818</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1812</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="3" t="s">
-        <v>1813</v>
+        <v>1820</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1814</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="3" t="s">
-        <v>1815</v>
+        <v>1822</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1814</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="3" t="s">
-        <v>1816</v>
+        <v>1823</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1814</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="3" t="s">
-        <v>1817</v>
+        <v>1824</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>1818</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="3" t="s">
-        <v>1819</v>
+        <v>1826</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1820</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="3" t="s">
-        <v>1400</v>
+        <v>1407</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1401</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="3" t="s">
-        <v>1821</v>
+        <v>1828</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1822</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="3" t="s">
-        <v>1823</v>
+        <v>1830</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1824</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="3" t="s">
-        <v>1825</v>
+        <v>1832</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1826</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="3" t="s">
-        <v>1827</v>
+        <v>1834</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>1828</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="3" t="s">
-        <v>1829</v>
+        <v>1836</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>1830</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="3" t="s">
-        <v>1398</v>
+        <v>1405</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>1399</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="3" t="s">
-        <v>1831</v>
+        <v>1838</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>1832</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="3" t="s">
-        <v>1833</v>
+        <v>1840</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1834</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="3" t="s">
-        <v>1835</v>
+        <v>1842</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>1836</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="3" t="s">
-        <v>1837</v>
+        <v>1844</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>1838</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="3" t="s">
-        <v>1839</v>
+        <v>1846</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>1840</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="3" t="s">
-        <v>1841</v>
+        <v>1848</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1842</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="3" t="s">
-        <v>1843</v>
+        <v>1850</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>1844</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="3" t="s">
-        <v>1845</v>
+        <v>1852</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>1846</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="3" t="s">
-        <v>1847</v>
+        <v>1854</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1848</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="3" t="s">
-        <v>1849</v>
+        <v>1856</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>1850</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="3" t="s">
-        <v>1851</v>
+        <v>1858</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>1852</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="3" t="s">
-        <v>1853</v>
+        <v>1860</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1854</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="3" t="s">
-        <v>1855</v>
+        <v>1862</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>1856</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="3" t="s">
-        <v>1857</v>
+        <v>1864</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>1858</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="3" t="s">
-        <v>1859</v>
+        <v>1866</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>1860</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="3" t="s">
-        <v>1861</v>
+        <v>1868</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>1862</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="3" t="s">
-        <v>1863</v>
+        <v>1870</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>1864</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="3" t="s">
-        <v>1865</v>
+        <v>1872</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>1866</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="3" t="s">
-        <v>1867</v>
+        <v>1874</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>1868</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="3" t="s">
-        <v>1869</v>
+        <v>1876</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1870</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="3" t="s">
-        <v>1871</v>
+        <v>1878</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>1872</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="3" t="s">
-        <v>1873</v>
+        <v>1880</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>1874</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="3" t="s">
-        <v>1875</v>
+        <v>1882</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>1876</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="3" t="s">
-        <v>1877</v>
+        <v>1884</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>1878</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="3" t="s">
-        <v>1879</v>
+        <v>1886</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>1880</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="3" t="s">
-        <v>1881</v>
+        <v>1888</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>1882</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="3" t="s">
-        <v>1883</v>
+        <v>1890</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>1848</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="3" t="s">
-        <v>1884</v>
+        <v>1891</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>1885</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="3" t="s">
-        <v>1886</v>
+        <v>1893</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>1887</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="3" t="s">
-        <v>1888</v>
+        <v>1895</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>1889</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="3" t="s">
-        <v>1890</v>
+        <v>1897</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1891</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="3" t="s">
-        <v>1892</v>
+        <v>1899</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>1893</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="3" t="s">
-        <v>1894</v>
+        <v>1901</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>1895</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="3" t="s">
-        <v>1896</v>
+        <v>1903</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>1897</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="3" t="s">
-        <v>1898</v>
+        <v>1905</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>1899</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="3" t="s">
-        <v>1900</v>
+        <v>1907</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>1901</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="3" t="s">
-        <v>1902</v>
+        <v>1909</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>1903</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="3" t="s">
-        <v>1904</v>
+        <v>1911</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>1905</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="3" t="s">
-        <v>1906</v>
+        <v>1913</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>1907</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="3" t="s">
-        <v>1908</v>
+        <v>1915</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>1909</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="3" t="s">
-        <v>1910</v>
+        <v>1917</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>1911</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="3" t="s">
-        <v>1402</v>
+        <v>1409</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>1403</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="3" t="s">
-        <v>1404</v>
+        <v>1411</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>1405</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="3" t="s">
-        <v>1406</v>
+        <v>1413</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>1407</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="3" t="s">
-        <v>1408</v>
+        <v>1415</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>1409</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="3" t="s">
-        <v>1410</v>
+        <v>1417</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>1411</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="3" t="s">
-        <v>1412</v>
+        <v>1419</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>1413</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="3" t="s">
-        <v>1414</v>
+        <v>1421</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>1415</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="3" t="s">
-        <v>1416</v>
+        <v>1423</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>1417</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="3" t="s">
-        <v>1418</v>
+        <v>1425</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>1419</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="3" t="s">
-        <v>1420</v>
+        <v>1427</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>1421</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="3" t="s">
-        <v>1422</v>
+        <v>1429</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>1423</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="3" t="s">
-        <v>1424</v>
+        <v>1431</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>1425</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="3" t="s">
-        <v>1426</v>
+        <v>1433</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>1427</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="3" t="s">
-        <v>1428</v>
+        <v>1435</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>1429</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="3" t="s">
-        <v>1430</v>
+        <v>1437</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>1431</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="3" t="s">
-        <v>1432</v>
+        <v>1439</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>1433</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="3" t="s">
-        <v>1912</v>
+        <v>1919</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>1913</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="3" t="s">
-        <v>1914</v>
+        <v>1921</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>1915</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="3" t="s">
-        <v>1916</v>
+        <v>1923</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>1917</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="3" t="s">
-        <v>1918</v>
+        <v>1925</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>1919</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="3" t="s">
-        <v>1920</v>
+        <v>1927</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>1921</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="3" t="s">
-        <v>1922</v>
+        <v>1929</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>1923</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="3" t="s">
-        <v>1924</v>
+        <v>1931</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>1925</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="3" t="s">
-        <v>1926</v>
+        <v>1933</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1927</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="3" t="s">
-        <v>1928</v>
+        <v>1935</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1929</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="3" t="s">
-        <v>1930</v>
+        <v>1937</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1931</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="3" t="s">
-        <v>1932</v>
+        <v>1939</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>1933</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="3" t="s">
-        <v>1934</v>
+        <v>1941</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>1935</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="3" t="s">
-        <v>1936</v>
+        <v>1943</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>1937</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="3" t="s">
-        <v>1938</v>
+        <v>1945</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>1939</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="3" t="s">
-        <v>1940</v>
+        <v>1947</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>1941</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="3" t="s">
-        <v>1942</v>
+        <v>1949</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>1943</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="3" t="s">
-        <v>1944</v>
+        <v>1951</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>1945</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="3" t="s">
-        <v>1946</v>
+        <v>1953</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>1947</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="3" t="s">
-        <v>1948</v>
+        <v>1955</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>1949</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="3" t="s">
-        <v>1950</v>
+        <v>1957</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>1951</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="3" t="s">
-        <v>1952</v>
+        <v>1959</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1953</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="3" t="s">
-        <v>1954</v>
+        <v>1961</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1955</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="3" t="s">
-        <v>1956</v>
+        <v>1963</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>1957</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="3" t="s">
-        <v>1958</v>
+        <v>1965</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1959</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="3" t="s">
-        <v>1960</v>
+        <v>1967</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1961</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="3" t="s">
-        <v>1962</v>
+        <v>1969</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>1963</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="3" t="s">
-        <v>1964</v>
+        <v>1971</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>1965</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="3" t="s">
-        <v>1966</v>
+        <v>1973</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>1967</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="3" t="s">
-        <v>1968</v>
+        <v>1975</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>1969</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="3" t="s">
-        <v>1970</v>
+        <v>1977</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>1971</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="3" t="s">
-        <v>1972</v>
+        <v>1979</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>1973</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="3" t="s">
-        <v>1974</v>
+        <v>1981</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>1975</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="3" t="s">
-        <v>1976</v>
+        <v>1983</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>1977</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="3" t="s">
-        <v>1978</v>
+        <v>1985</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>1979</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="3" t="s">
-        <v>1980</v>
+        <v>1987</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>1981</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="3" t="s">
-        <v>1982</v>
+        <v>1989</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>1983</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="3" t="s">
-        <v>1984</v>
+        <v>1991</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>1985</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="3" t="s">
-        <v>1986</v>
+        <v>1993</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>1987</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="3" t="s">
-        <v>1988</v>
+        <v>1995</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>1989</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="3" t="s">
-        <v>1990</v>
+        <v>1997</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>1991</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="3" t="s">
-        <v>1992</v>
+        <v>1999</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>1993</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="3" t="s">
-        <v>1994</v>
+        <v>2001</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>1995</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="3" t="s">
-        <v>1996</v>
+        <v>2003</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>1997</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="3" t="s">
-        <v>1998</v>
+        <v>2005</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>1993</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="3" t="s">
-        <v>1999</v>
+        <v>2006</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>1995</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="3" t="s">
-        <v>2000</v>
+        <v>2007</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>2001</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="3" t="s">
-        <v>2002</v>
+        <v>2009</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>1993</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="3" t="s">
-        <v>2003</v>
+        <v>2010</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>1995</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="3" t="s">
-        <v>2004</v>
+        <v>2011</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>2005</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="3" t="s">
-        <v>2006</v>
+        <v>2013</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>1993</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="3" t="s">
-        <v>2007</v>
+        <v>2014</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>1995</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="3" t="s">
-        <v>2008</v>
+        <v>2015</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>2009</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="3" t="s">
-        <v>2010</v>
+        <v>2017</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>1993</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="3" t="s">
-        <v>2011</v>
+        <v>2018</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>1995</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="3" t="s">
-        <v>2012</v>
+        <v>2019</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>2013</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="3" t="s">
-        <v>2014</v>
+        <v>2021</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>1993</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="3" t="s">
-        <v>2015</v>
+        <v>2022</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>1995</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="3" t="s">
-        <v>2016</v>
+        <v>2023</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>2017</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="3" t="s">
-        <v>2018</v>
+        <v>2025</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1993</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="3" t="s">
-        <v>2019</v>
+        <v>2026</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>1995</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="3" t="s">
-        <v>2020</v>
+        <v>2027</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>2021</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="3" t="s">
-        <v>2022</v>
+        <v>2029</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>1993</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="3" t="s">
-        <v>2023</v>
+        <v>2030</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>1995</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="3" t="s">
-        <v>2024</v>
+        <v>2031</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>2025</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="3" t="s">
-        <v>2026</v>
+        <v>2033</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>1826</v>
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="4" t="s">
+        <v>2034</v>
+      </c>
+      <c r="B334" s="4" t="s">
+        <v>2035</v>
       </c>
     </row>
   </sheetData>
@@ -21356,10 +21415,10 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>2027</v>
+        <v>2036</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2028</v>
+        <v>2037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualización para selección de nombres
Empezar las variables de tasas con "ta."
</commit_message>
<xml_diff>
--- a/Tasas/caja/caja.xlsx
+++ b/Tasas/caja/caja.xlsx
@@ -993,7 +993,7 @@
     <t>2018</t>
   </si>
   <si>
-    <t>mh_colNo.aplica_y2017.2018</t>
+    <t>ta.mh_colNo.aplica_y2017.2018</t>
   </si>
   <si>
     <t>mh_colNo.aplica_y2019</t>
@@ -1005,7 +1005,7 @@
     <t>2019</t>
   </si>
   <si>
-    <t>mh_colNo.aplica_y2018.2019</t>
+    <t>ta.mh_colNo.aplica_y2018.2019</t>
   </si>
   <si>
     <t>mh_colNo.aplica_y2020</t>
@@ -1017,7 +1017,7 @@
     <t>2020</t>
   </si>
   <si>
-    <t>mh_colNo.aplica_y2019.2020</t>
+    <t>ta.mh_colNo.aplica_y2019.2020</t>
   </si>
   <si>
     <t>mh_colNo.aplica_y2021</t>
@@ -1029,7 +1029,7 @@
     <t>2021</t>
   </si>
   <si>
-    <t>mh_colNo.aplica_y2020.2021</t>
+    <t>ta.mh_colNo.aplica_y2020.2021</t>
   </si>
   <si>
     <t>mh_colNo.aplica_y2022</t>
@@ -1041,7 +1041,7 @@
     <t>2022</t>
   </si>
   <si>
-    <t>mh_colNo.aplica_y2021.2022</t>
+    <t>ta.mh_colNo.aplica_y2021.2022</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2017</t>
@@ -1050,31 +1050,31 @@
     <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2018</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2017.2018</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2017.2018</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2019</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2018.2019</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2018.2019</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2020</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2019.2020</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2019.2020</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2021</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2020.2021</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2020.2021</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2022</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2021.2022</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Asalariados.INFORMALES_y2021.2022</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2017</t>
@@ -1083,31 +1083,31 @@
     <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2018</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2017.2018</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2017.2018</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2019</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2018.2019</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2018.2019</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2020</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2019.2020</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2019.2020</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2021</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2020.2021</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2020.2021</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2022</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2021.2022</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Asalariados.FORMALES_y2021.2022</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2017</t>
@@ -1116,31 +1116,31 @@
     <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2018</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2017.2018</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2017.2018</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2019</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2018.2019</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2018.2019</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2020</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2019.2020</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2019.2020</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2021</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2020.2021</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2020.2021</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2022</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2021.2022</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.INFORMALES_y2021.2022</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2017</t>
@@ -1149,31 +1149,31 @@
     <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2018</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2017.2018</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2017.2018</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2019</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2018.2019</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2018.2019</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2020</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2019.2020</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2019.2020</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2021</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2020.2021</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2020.2021</t>
   </si>
   <si>
     <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2022</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2021.2022</t>
+    <t>ta.mh_colTrabajadores.subordinados.y.remunerados...Con.percepciones.no.salariales.FORMALES_y2021.2022</t>
   </si>
   <si>
     <t>mh_colEmpleadores.INFORMAL_y2017</t>
@@ -1182,31 +1182,31 @@
     <t>mh_colEmpleadores.INFORMAL_y2018</t>
   </si>
   <si>
-    <t>mh_colEmpleadores.INFORMAL_y2017.2018</t>
+    <t>ta.mh_colEmpleadores.INFORMAL_y2017.2018</t>
   </si>
   <si>
     <t>mh_colEmpleadores.INFORMAL_y2019</t>
   </si>
   <si>
-    <t>mh_colEmpleadores.INFORMAL_y2018.2019</t>
+    <t>ta.mh_colEmpleadores.INFORMAL_y2018.2019</t>
   </si>
   <si>
     <t>mh_colEmpleadores.INFORMAL_y2020</t>
   </si>
   <si>
-    <t>mh_colEmpleadores.INFORMAL_y2019.2020</t>
+    <t>ta.mh_colEmpleadores.INFORMAL_y2019.2020</t>
   </si>
   <si>
     <t>mh_colEmpleadores.INFORMAL_y2021</t>
   </si>
   <si>
-    <t>mh_colEmpleadores.INFORMAL_y2020.2021</t>
+    <t>ta.mh_colEmpleadores.INFORMAL_y2020.2021</t>
   </si>
   <si>
     <t>mh_colEmpleadores.INFORMAL_y2022</t>
   </si>
   <si>
-    <t>mh_colEmpleadores.INFORMAL_y2021.2022</t>
+    <t>ta.mh_colEmpleadores.INFORMAL_y2021.2022</t>
   </si>
   <si>
     <t>mh_colEmpleadores.FORMAL_y2017</t>
@@ -1215,31 +1215,31 @@
     <t>mh_colEmpleadores.FORMAL_y2018</t>
   </si>
   <si>
-    <t>mh_colEmpleadores.FORMAL_y2017.2018</t>
+    <t>ta.mh_colEmpleadores.FORMAL_y2017.2018</t>
   </si>
   <si>
     <t>mh_colEmpleadores.FORMAL_y2019</t>
   </si>
   <si>
-    <t>mh_colEmpleadores.FORMAL_y2018.2019</t>
+    <t>ta.mh_colEmpleadores.FORMAL_y2018.2019</t>
   </si>
   <si>
     <t>mh_colEmpleadores.FORMAL_y2020</t>
   </si>
   <si>
-    <t>mh_colEmpleadores.FORMAL_y2019.2020</t>
+    <t>ta.mh_colEmpleadores.FORMAL_y2019.2020</t>
   </si>
   <si>
     <t>mh_colEmpleadores.FORMAL_y2021</t>
   </si>
   <si>
-    <t>mh_colEmpleadores.FORMAL_y2020.2021</t>
+    <t>ta.mh_colEmpleadores.FORMAL_y2020.2021</t>
   </si>
   <si>
     <t>mh_colEmpleadores.FORMAL_y2022</t>
   </si>
   <si>
-    <t>mh_colEmpleadores.FORMAL_y2021.2022</t>
+    <t>ta.mh_colEmpleadores.FORMAL_y2021.2022</t>
   </si>
   <si>
     <t>mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2017</t>
@@ -1248,31 +1248,31 @@
     <t>mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2018</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2017.2018</t>
+    <t>ta.mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2017.2018</t>
   </si>
   <si>
     <t>mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2019</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2018.2019</t>
+    <t>ta.mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2018.2019</t>
   </si>
   <si>
     <t>mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2020</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2019.2020</t>
+    <t>ta.mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2019.2020</t>
   </si>
   <si>
     <t>mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2021</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2020.2021</t>
+    <t>ta.mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2020.2021</t>
   </si>
   <si>
     <t>mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2022</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2021.2022</t>
+    <t>ta.mh_colTrabajadores.por.cuenta.propia.INFORMAL_y2021.2022</t>
   </si>
   <si>
     <t>mh_colTrabajadores.por.cuenta.propia.FORMAL_y2017</t>
@@ -1281,31 +1281,31 @@
     <t>mh_colTrabajadores.por.cuenta.propia.FORMAL_y2018</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.por.cuenta.propia.FORMAL_y2017.2018</t>
+    <t>ta.mh_colTrabajadores.por.cuenta.propia.FORMAL_y2017.2018</t>
   </si>
   <si>
     <t>mh_colTrabajadores.por.cuenta.propia.FORMAL_y2019</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.por.cuenta.propia.FORMAL_y2018.2019</t>
+    <t>ta.mh_colTrabajadores.por.cuenta.propia.FORMAL_y2018.2019</t>
   </si>
   <si>
     <t>mh_colTrabajadores.por.cuenta.propia.FORMAL_y2020</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.por.cuenta.propia.FORMAL_y2019.2020</t>
+    <t>ta.mh_colTrabajadores.por.cuenta.propia.FORMAL_y2019.2020</t>
   </si>
   <si>
     <t>mh_colTrabajadores.por.cuenta.propia.FORMAL_y2021</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.por.cuenta.propia.FORMAL_y2020.2021</t>
+    <t>ta.mh_colTrabajadores.por.cuenta.propia.FORMAL_y2020.2021</t>
   </si>
   <si>
     <t>mh_colTrabajadores.por.cuenta.propia.FORMAL_y2022</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.por.cuenta.propia.FORMAL_y2021.2022</t>
+    <t>ta.mh_colTrabajadores.por.cuenta.propia.FORMAL_y2021.2022</t>
   </si>
   <si>
     <t>mh_colTrabajadores.no.Remunerados.INFORMAL_y2017</t>
@@ -1314,31 +1314,31 @@
     <t>mh_colTrabajadores.no.Remunerados.INFORMAL_y2018</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.no.Remunerados.INFORMAL_y2017.2018</t>
+    <t>ta.mh_colTrabajadores.no.Remunerados.INFORMAL_y2017.2018</t>
   </si>
   <si>
     <t>mh_colTrabajadores.no.Remunerados.INFORMAL_y2019</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.no.Remunerados.INFORMAL_y2018.2019</t>
+    <t>ta.mh_colTrabajadores.no.Remunerados.INFORMAL_y2018.2019</t>
   </si>
   <si>
     <t>mh_colTrabajadores.no.Remunerados.INFORMAL_y2020</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.no.Remunerados.INFORMAL_y2019.2020</t>
+    <t>ta.mh_colTrabajadores.no.Remunerados.INFORMAL_y2019.2020</t>
   </si>
   <si>
     <t>mh_colTrabajadores.no.Remunerados.INFORMAL_y2021</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.no.Remunerados.INFORMAL_y2020.2021</t>
+    <t>ta.mh_colTrabajadores.no.Remunerados.INFORMAL_y2020.2021</t>
   </si>
   <si>
     <t>mh_colTrabajadores.no.Remunerados.INFORMAL_y2022</t>
   </si>
   <si>
-    <t>mh_colTrabajadores.no.Remunerados.INFORMAL_y2021.2022</t>
+    <t>ta.mh_colTrabajadores.no.Remunerados.INFORMAL_y2021.2022</t>
   </si>
   <si>
     <t>rama_est2No.aplica_y2017</t>
@@ -1347,31 +1347,31 @@
     <t>rama_est2No.aplica_y2018</t>
   </si>
   <si>
-    <t>rama_est2No.aplica_y2017.2018</t>
+    <t>ta.rama_est2No.aplica_y2017.2018</t>
   </si>
   <si>
     <t>rama_est2No.aplica_y2019</t>
   </si>
   <si>
-    <t>rama_est2No.aplica_y2018.2019</t>
+    <t>ta.rama_est2No.aplica_y2018.2019</t>
   </si>
   <si>
     <t>rama_est2No.aplica_y2020</t>
   </si>
   <si>
-    <t>rama_est2No.aplica_y2019.2020</t>
+    <t>ta.rama_est2No.aplica_y2019.2020</t>
   </si>
   <si>
     <t>rama_est2No.aplica_y2021</t>
   </si>
   <si>
-    <t>rama_est2No.aplica_y2020.2021</t>
+    <t>ta.rama_est2No.aplica_y2020.2021</t>
   </si>
   <si>
     <t>rama_est2No.aplica_y2022</t>
   </si>
   <si>
-    <t>rama_est2No.aplica_y2021.2022</t>
+    <t>ta.rama_est2No.aplica_y2021.2022</t>
   </si>
   <si>
     <t>rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2017</t>
@@ -1380,31 +1380,31 @@
     <t>rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2018</t>
   </si>
   <si>
-    <t>rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2017.2018</t>
+    <t>ta.rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2017.2018</t>
   </si>
   <si>
     <t>rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2019</t>
   </si>
   <si>
-    <t>rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2018.2019</t>
+    <t>ta.rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2018.2019</t>
   </si>
   <si>
     <t>rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2020</t>
   </si>
   <si>
-    <t>rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2019.2020</t>
+    <t>ta.rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2019.2020</t>
   </si>
   <si>
     <t>rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2021</t>
   </si>
   <si>
-    <t>rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2020.2021</t>
+    <t>ta.rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2020.2021</t>
   </si>
   <si>
     <t>rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2022</t>
   </si>
   <si>
-    <t>rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2021.2022</t>
+    <t>ta.rama_est2Agricultura..ganadería..silvicultura..caza.y.pesca_y2021.2022</t>
   </si>
   <si>
     <t>rama_est2Industria.extractiva.y.de.la.electricidad_y2017</t>
@@ -1413,31 +1413,31 @@
     <t>rama_est2Industria.extractiva.y.de.la.electricidad_y2018</t>
   </si>
   <si>
-    <t>rama_est2Industria.extractiva.y.de.la.electricidad_y2017.2018</t>
+    <t>ta.rama_est2Industria.extractiva.y.de.la.electricidad_y2017.2018</t>
   </si>
   <si>
     <t>rama_est2Industria.extractiva.y.de.la.electricidad_y2019</t>
   </si>
   <si>
-    <t>rama_est2Industria.extractiva.y.de.la.electricidad_y2018.2019</t>
+    <t>ta.rama_est2Industria.extractiva.y.de.la.electricidad_y2018.2019</t>
   </si>
   <si>
     <t>rama_est2Industria.extractiva.y.de.la.electricidad_y2020</t>
   </si>
   <si>
-    <t>rama_est2Industria.extractiva.y.de.la.electricidad_y2019.2020</t>
+    <t>ta.rama_est2Industria.extractiva.y.de.la.electricidad_y2019.2020</t>
   </si>
   <si>
     <t>rama_est2Industria.extractiva.y.de.la.electricidad_y2021</t>
   </si>
   <si>
-    <t>rama_est2Industria.extractiva.y.de.la.electricidad_y2020.2021</t>
+    <t>ta.rama_est2Industria.extractiva.y.de.la.electricidad_y2020.2021</t>
   </si>
   <si>
     <t>rama_est2Industria.extractiva.y.de.la.electricidad_y2022</t>
   </si>
   <si>
-    <t>rama_est2Industria.extractiva.y.de.la.electricidad_y2021.2022</t>
+    <t>ta.rama_est2Industria.extractiva.y.de.la.electricidad_y2021.2022</t>
   </si>
   <si>
     <t>rama_est2Industria.manufacturera_y2017</t>
@@ -1446,31 +1446,31 @@
     <t>rama_est2Industria.manufacturera_y2018</t>
   </si>
   <si>
-    <t>rama_est2Industria.manufacturera_y2017.2018</t>
+    <t>ta.rama_est2Industria.manufacturera_y2017.2018</t>
   </si>
   <si>
     <t>rama_est2Industria.manufacturera_y2019</t>
   </si>
   <si>
-    <t>rama_est2Industria.manufacturera_y2018.2019</t>
+    <t>ta.rama_est2Industria.manufacturera_y2018.2019</t>
   </si>
   <si>
     <t>rama_est2Industria.manufacturera_y2020</t>
   </si>
   <si>
-    <t>rama_est2Industria.manufacturera_y2019.2020</t>
+    <t>ta.rama_est2Industria.manufacturera_y2019.2020</t>
   </si>
   <si>
     <t>rama_est2Industria.manufacturera_y2021</t>
   </si>
   <si>
-    <t>rama_est2Industria.manufacturera_y2020.2021</t>
+    <t>ta.rama_est2Industria.manufacturera_y2020.2021</t>
   </si>
   <si>
     <t>rama_est2Industria.manufacturera_y2022</t>
   </si>
   <si>
-    <t>rama_est2Industria.manufacturera_y2021.2022</t>
+    <t>ta.rama_est2Industria.manufacturera_y2021.2022</t>
   </si>
   <si>
     <t>rama_est2Construcción_y2017</t>
@@ -1479,31 +1479,31 @@
     <t>rama_est2Construcción_y2018</t>
   </si>
   <si>
-    <t>rama_est2Construcción_y2017.2018</t>
+    <t>ta.rama_est2Construcción_y2017.2018</t>
   </si>
   <si>
     <t>rama_est2Construcción_y2019</t>
   </si>
   <si>
-    <t>rama_est2Construcción_y2018.2019</t>
+    <t>ta.rama_est2Construcción_y2018.2019</t>
   </si>
   <si>
     <t>rama_est2Construcción_y2020</t>
   </si>
   <si>
-    <t>rama_est2Construcción_y2019.2020</t>
+    <t>ta.rama_est2Construcción_y2019.2020</t>
   </si>
   <si>
     <t>rama_est2Construcción_y2021</t>
   </si>
   <si>
-    <t>rama_est2Construcción_y2020.2021</t>
+    <t>ta.rama_est2Construcción_y2020.2021</t>
   </si>
   <si>
     <t>rama_est2Construcción_y2022</t>
   </si>
   <si>
-    <t>rama_est2Construcción_y2021.2022</t>
+    <t>ta.rama_est2Construcción_y2021.2022</t>
   </si>
   <si>
     <t>rama_est2Comercio_y2017</t>
@@ -1512,31 +1512,31 @@
     <t>rama_est2Comercio_y2018</t>
   </si>
   <si>
-    <t>rama_est2Comercio_y2017.2018</t>
+    <t>ta.rama_est2Comercio_y2017.2018</t>
   </si>
   <si>
     <t>rama_est2Comercio_y2019</t>
   </si>
   <si>
-    <t>rama_est2Comercio_y2018.2019</t>
+    <t>ta.rama_est2Comercio_y2018.2019</t>
   </si>
   <si>
     <t>rama_est2Comercio_y2020</t>
   </si>
   <si>
-    <t>rama_est2Comercio_y2019.2020</t>
+    <t>ta.rama_est2Comercio_y2019.2020</t>
   </si>
   <si>
     <t>rama_est2Comercio_y2021</t>
   </si>
   <si>
-    <t>rama_est2Comercio_y2020.2021</t>
+    <t>ta.rama_est2Comercio_y2020.2021</t>
   </si>
   <si>
     <t>rama_est2Comercio_y2022</t>
   </si>
   <si>
-    <t>rama_est2Comercio_y2021.2022</t>
+    <t>ta.rama_est2Comercio_y2021.2022</t>
   </si>
   <si>
     <t>rama_est2Restaurantes.y.servicios.de.alojamiento_y2017</t>
@@ -1545,31 +1545,31 @@
     <t>rama_est2Restaurantes.y.servicios.de.alojamiento_y2018</t>
   </si>
   <si>
-    <t>rama_est2Restaurantes.y.servicios.de.alojamiento_y2017.2018</t>
+    <t>ta.rama_est2Restaurantes.y.servicios.de.alojamiento_y2017.2018</t>
   </si>
   <si>
     <t>rama_est2Restaurantes.y.servicios.de.alojamiento_y2019</t>
   </si>
   <si>
-    <t>rama_est2Restaurantes.y.servicios.de.alojamiento_y2018.2019</t>
+    <t>ta.rama_est2Restaurantes.y.servicios.de.alojamiento_y2018.2019</t>
   </si>
   <si>
     <t>rama_est2Restaurantes.y.servicios.de.alojamiento_y2020</t>
   </si>
   <si>
-    <t>rama_est2Restaurantes.y.servicios.de.alojamiento_y2019.2020</t>
+    <t>ta.rama_est2Restaurantes.y.servicios.de.alojamiento_y2019.2020</t>
   </si>
   <si>
     <t>rama_est2Restaurantes.y.servicios.de.alojamiento_y2021</t>
   </si>
   <si>
-    <t>rama_est2Restaurantes.y.servicios.de.alojamiento_y2020.2021</t>
+    <t>ta.rama_est2Restaurantes.y.servicios.de.alojamiento_y2020.2021</t>
   </si>
   <si>
     <t>rama_est2Restaurantes.y.servicios.de.alojamiento_y2022</t>
   </si>
   <si>
-    <t>rama_est2Restaurantes.y.servicios.de.alojamiento_y2021.2022</t>
+    <t>ta.rama_est2Restaurantes.y.servicios.de.alojamiento_y2021.2022</t>
   </si>
   <si>
     <t>rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2017</t>
@@ -1578,37 +1578,37 @@
     <t>rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2018</t>
   </si>
   <si>
-    <t>rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2017.2018</t>
+    <t>ta.rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2017.2018</t>
   </si>
   <si>
     <t>rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2019</t>
   </si>
   <si>
-    <t>rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2018.2019</t>
+    <t>ta.rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2018.2019</t>
   </si>
   <si>
     <t>rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2020</t>
   </si>
   <si>
-    <t>rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2019.2020</t>
+    <t>ta.rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2019.2020</t>
   </si>
   <si>
     <t>rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2021</t>
   </si>
   <si>
-    <t>rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2020.2021</t>
+    <t>ta.rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2020.2021</t>
   </si>
   <si>
     <t>rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2022</t>
   </si>
   <si>
-    <t>rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2021.2022</t>
+    <t>ta.rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2021.2022</t>
   </si>
   <si>
     <t>rama_est2Servicios.profesionales..financieros.y.corporativos_y2017</t>
   </si>
   <si>
-    <t>rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2022.2018</t>
+    <t>ta.rama_est2Transportes..comunicaciones..correo.y.almacenamiento_y2022.2018</t>
   </si>
   <si>
     <t>rama_est2Servicios.profesionales..financieros.y.corporativos_y2018</t>
@@ -1617,25 +1617,25 @@
     <t>rama_est2Servicios.profesionales..financieros.y.corporativos_y2019</t>
   </si>
   <si>
-    <t>rama_est2Servicios.profesionales..financieros.y.corporativos_y2018.2019</t>
+    <t>ta.rama_est2Servicios.profesionales..financieros.y.corporativos_y2018.2019</t>
   </si>
   <si>
     <t>rama_est2Servicios.profesionales..financieros.y.corporativos_y2020</t>
   </si>
   <si>
-    <t>rama_est2Servicios.profesionales..financieros.y.corporativos_y2019.2020</t>
+    <t>ta.rama_est2Servicios.profesionales..financieros.y.corporativos_y2019.2020</t>
   </si>
   <si>
     <t>rama_est2Servicios.profesionales..financieros.y.corporativos_y2021</t>
   </si>
   <si>
-    <t>rama_est2Servicios.profesionales..financieros.y.corporativos_y2020.2021</t>
+    <t>ta.rama_est2Servicios.profesionales..financieros.y.corporativos_y2020.2021</t>
   </si>
   <si>
     <t>rama_est2Servicios.profesionales..financieros.y.corporativos_y2022</t>
   </si>
   <si>
-    <t>rama_est2Servicios.profesionales..financieros.y.corporativos_y2021.2022</t>
+    <t>ta.rama_est2Servicios.profesionales..financieros.y.corporativos_y2021.2022</t>
   </si>
   <si>
     <t>rama_est2Servicios.sociales_y2017</t>
@@ -1644,31 +1644,31 @@
     <t>rama_est2Servicios.sociales_y2018</t>
   </si>
   <si>
-    <t>rama_est2Servicios.sociales_y2017.2018</t>
+    <t>ta.rama_est2Servicios.sociales_y2017.2018</t>
   </si>
   <si>
     <t>rama_est2Servicios.sociales_y2019</t>
   </si>
   <si>
-    <t>rama_est2Servicios.sociales_y2018.2019</t>
+    <t>ta.rama_est2Servicios.sociales_y2018.2019</t>
   </si>
   <si>
     <t>rama_est2Servicios.sociales_y2020</t>
   </si>
   <si>
-    <t>rama_est2Servicios.sociales_y2019.2020</t>
+    <t>ta.rama_est2Servicios.sociales_y2019.2020</t>
   </si>
   <si>
     <t>rama_est2Servicios.sociales_y2021</t>
   </si>
   <si>
-    <t>rama_est2Servicios.sociales_y2020.2021</t>
+    <t>ta.rama_est2Servicios.sociales_y2020.2021</t>
   </si>
   <si>
     <t>rama_est2Servicios.sociales_y2022</t>
   </si>
   <si>
-    <t>rama_est2Servicios.sociales_y2021.2022</t>
+    <t>ta.rama_est2Servicios.sociales_y2021.2022</t>
   </si>
   <si>
     <t>rama_est2Servicios.diversos_y2017</t>
@@ -1677,31 +1677,31 @@
     <t>rama_est2Servicios.diversos_y2018</t>
   </si>
   <si>
-    <t>rama_est2Servicios.diversos_y2017.2018</t>
+    <t>ta.rama_est2Servicios.diversos_y2017.2018</t>
   </si>
   <si>
     <t>rama_est2Servicios.diversos_y2019</t>
   </si>
   <si>
-    <t>rama_est2Servicios.diversos_y2018.2019</t>
+    <t>ta.rama_est2Servicios.diversos_y2018.2019</t>
   </si>
   <si>
     <t>rama_est2Servicios.diversos_y2020</t>
   </si>
   <si>
-    <t>rama_est2Servicios.diversos_y2019.2020</t>
+    <t>ta.rama_est2Servicios.diversos_y2019.2020</t>
   </si>
   <si>
     <t>rama_est2Servicios.diversos_y2021</t>
   </si>
   <si>
-    <t>rama_est2Servicios.diversos_y2020.2021</t>
+    <t>ta.rama_est2Servicios.diversos_y2020.2021</t>
   </si>
   <si>
     <t>rama_est2Servicios.diversos_y2022</t>
   </si>
   <si>
-    <t>rama_est2Servicios.diversos_y2021.2022</t>
+    <t>ta.rama_est2Servicios.diversos_y2021.2022</t>
   </si>
   <si>
     <t>rama_est2Gobierno.y.organismos.internacionales_y2017</t>
@@ -1710,52 +1710,52 @@
     <t>rama_est2Gobierno.y.organismos.internacionales_y2018</t>
   </si>
   <si>
-    <t>rama_est2Gobierno.y.organismos.internacionales_y2017.2018</t>
+    <t>ta.rama_est2Gobierno.y.organismos.internacionales_y2017.2018</t>
   </si>
   <si>
     <t>rama_est2Gobierno.y.organismos.internacionales_y2019</t>
   </si>
   <si>
-    <t>rama_est2Gobierno.y.organismos.internacionales_y2018.2019</t>
+    <t>ta.rama_est2Gobierno.y.organismos.internacionales_y2018.2019</t>
   </si>
   <si>
     <t>rama_est2Gobierno.y.organismos.internacionales_y2020</t>
   </si>
   <si>
-    <t>rama_est2Gobierno.y.organismos.internacionales_y2019.2020</t>
+    <t>ta.rama_est2Gobierno.y.organismos.internacionales_y2019.2020</t>
   </si>
   <si>
     <t>rama_est2Gobierno.y.organismos.internacionales_y2021</t>
   </si>
   <si>
-    <t>rama_est2Gobierno.y.organismos.internacionales_y2020.2021</t>
+    <t>ta.rama_est2Gobierno.y.organismos.internacionales_y2020.2021</t>
   </si>
   <si>
     <t>rama_est2Gobierno.y.organismos.internacionales_y2022</t>
   </si>
   <si>
-    <t>rama_est2Gobierno.y.organismos.internacionales_y2021.2022</t>
+    <t>ta.rama_est2Gobierno.y.organismos.internacionales_y2021.2022</t>
   </si>
   <si>
     <t>Tamaño</t>
   </si>
   <si>
-    <t>n_y2017.2018</t>
-  </si>
-  <si>
-    <t>n_y2018.2019</t>
-  </si>
-  <si>
-    <t>n_y2019.2020</t>
-  </si>
-  <si>
-    <t>n_y2020.2021</t>
+    <t>ta.n_y2017.2018</t>
+  </si>
+  <si>
+    <t>ta.n_y2018.2019</t>
+  </si>
+  <si>
+    <t>ta.n_y2019.2020</t>
+  </si>
+  <si>
+    <t>ta.n_y2020.2021</t>
   </si>
   <si>
     <t>n_y2022</t>
   </si>
   <si>
-    <t>n_y2021.2022</t>
+    <t>ta.n_y2021.2022</t>
   </si>
   <si>
     <t>arch</t>

</xml_diff>